<commit_message>
collision manager bug fix + object interaction by range
</commit_message>
<xml_diff>
--- a/Engine/data/player_parameter.xlsx
+++ b/Engine/data/player_parameter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\js_choi\Desktop\mainproject\Engine\Engine\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4740AED-E122-4DEF-A845-12DA463742FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFED595B-2383-410E-99D3-99D6AF178C65}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1048,7 +1048,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1276,7 +1276,7 @@
         <v>22</v>
       </c>
       <c r="B20">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C20" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
[refactor] graphicsclass calling gm frame
</commit_message>
<xml_diff>
--- a/Engine/data/player_parameter.xlsx
+++ b/Engine/data/player_parameter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\js_choi\Desktop\mainproject\Engine\Engine\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFED595B-2383-410E-99D3-99D6AF178C65}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA587131-809E-48DA-969B-56B4C1E0BF14}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5835" yWindow="3945" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="player_parameter" sheetId="1" r:id="rId1"/>
@@ -1048,7 +1048,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1155,7 +1155,7 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -1166,7 +1166,7 @@
         <v>12</v>
       </c>
       <c r="B10">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>

</xml_diff>